<commit_message>
change hoehe to anzahl in wackelturn
</commit_message>
<xml_diff>
--- a/BavarianGames.xlsx
+++ b/BavarianGames.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Gruppe" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
     <sheet name="PktBulldogziehen" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="PktBierkruglauf" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="R1C1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">T4_V3</t>
   </si>
   <si>
-    <t xml:space="preserve">Hoehe</t>
+    <t xml:space="preserve">Anzahl</t>
   </si>
   <si>
     <t xml:space="preserve">T1</t>
@@ -526,8 +526,8 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -786,65 +786,65 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>10000</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>5000</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>120</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>5000</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>3780</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove calculation of Bierkruglauf
</commit_message>
<xml_diff>
--- a/BavarianGames.xlsx
+++ b/BavarianGames.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Gruppe" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
     <sheet name="PktBulldogziehen" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="PktBierkruglauf" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="R1C1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t xml:space="preserve">GruppenID</t>
   </si>
@@ -127,10 +127,7 @@
     <t xml:space="preserve">Zeit</t>
   </si>
   <si>
-    <t xml:space="preserve">Pkt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StrafPkt</t>
+    <t xml:space="preserve">Gesamt</t>
   </si>
 </sst>
 </file>
@@ -526,7 +523,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -786,8 +783,8 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -799,12 +796,8 @@
       <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -813,12 +806,8 @@
       <c r="B2" s="1" t="n">
         <v>10000</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>5000</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>120</v>
-      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -827,12 +816,8 @@
       <c r="B3" s="1" t="n">
         <v>5000</v>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>100</v>
-      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -841,12 +826,8 @@
       <c r="B4" s="1" t="n">
         <v>3780</v>
       </c>
-      <c r="C4" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>120</v>
-      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
same gesamt case added masskrugschieben
</commit_message>
<xml_diff>
--- a/BavarianGames.xlsx
+++ b/BavarianGames.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Gruppe" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
     <sheet name="PktBulldogziehen" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="PktBierkruglauf" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="R1C1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -335,8 +335,8 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -461,7 +461,7 @@
         <v>100</v>
       </c>
       <c r="M3" s="1" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -783,7 +783,7 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>